<commit_message>
clean metadata from Excel files we created
</commit_message>
<xml_diff>
--- a/data/240801 ISO3-ISO2-codes.xlsx
+++ b/data/240801 ISO3-ISO2-codes.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwaidelich\Downloads\GitHub - Local\eca_energyfinance\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86528505-1DC1-45BB-BEB1-D747A746EEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA2C91D-BF34-4B0D-B2AF-5E97762017E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D5E63907-5956-4B85-886C-BB7BFACE2043}"/>
+    <workbookView xWindow="-28920" yWindow="-3330" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D5E63907-5956-4B85-886C-BB7BFACE2043}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="2" r:id="rId1"/>
@@ -2774,7 +2769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0320C74-D488-4D2C-B107-0C1420FDDDE7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2806,6 +2801,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2813,9 +2809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C9AA43-8360-487C-8E7E-ED64A1CEB87F}">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -3645,7 +3639,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1">
+    <row r="60" spans="1:4" ht="20.5" thickBot="1">
       <c r="A60" s="1" t="s">
         <v>178</v>
       </c>
@@ -5717,7 +5711,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="50.5" thickBot="1">
+    <row r="208" spans="1:4" ht="60.5" thickBot="1">
       <c r="A208" s="1" t="s">
         <v>622</v>
       </c>
@@ -6321,5 +6315,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>